<commit_message>
Change algorythm now works!
</commit_message>
<xml_diff>
--- a/DocFilesFillingProgramm/DocFilesFillingProgrammConsoleTest/bin/Debug/Storage/excelStorage.xlsx
+++ b/DocFilesFillingProgramm/DocFilesFillingProgrammConsoleTest/bin/Debug/Storage/excelStorage.xlsx
@@ -229,45 +229,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
-    <t>BIRTHDATE</t>
-  </si>
-  <si>
-    <t>BEGINDATE</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
-    <t>GERMARK</t>
-  </si>
-  <si>
-    <t>UKRMARK</t>
-  </si>
-  <si>
-    <t>FILLDATE</t>
-  </si>
-  <si>
-    <t>GENDER</t>
-  </si>
-  <si>
-    <t>DL</t>
-  </si>
-  <si>
-    <t>DN</t>
-  </si>
-  <si>
-    <t>HD</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
     <t>UKR MARKS</t>
   </si>
   <si>
@@ -319,12 +283,6 @@
     <t>180</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kostantin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kovalenko</t>
-  </si>
-  <si>
     <t>23.05.1995</t>
   </si>
   <si>
@@ -361,10 +319,52 @@
     <t>181</t>
   </si>
   <si>
-    <t>Petrenko</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ivan</t>
+    <t>ukrmark</t>
+  </si>
+  <si>
+    <t>germark</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>dl</t>
+  </si>
+  <si>
+    <t>dn</t>
+  </si>
+  <si>
+    <t>filldate</t>
+  </si>
+  <si>
+    <t>hd</t>
+  </si>
+  <si>
+    <t>md</t>
+  </si>
+  <si>
+    <t>enddate</t>
+  </si>
+  <si>
+    <t>begindate</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>KONSTANTIN</t>
+  </si>
+  <si>
+    <t>DARYA</t>
+  </si>
+  <si>
+    <t>KOVALENKO</t>
+  </si>
+  <si>
+    <t>BLABLABLA</t>
   </si>
 </sst>
 </file>
@@ -778,12 +778,12 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -798,87 +798,87 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="K2" s="9">
         <v>2</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="N2" s="9">
         <v>45</v>
@@ -886,43 +886,43 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="D3" s="9" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="K3" s="9">
         <v>3</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="N3" s="9">
         <v>46</v>
@@ -989,33 +989,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -1023,16 +1023,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -1040,13 +1040,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E4" s="6"/>
     </row>

</xml_diff>